<commit_message>
fixing bug format exel
</commit_message>
<xml_diff>
--- a/public/templates/Book1.xlsx
+++ b/public/templates/Book1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc 40\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FA8D51-5AAC-4C51-8D69-FB5C8014A6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03B19483-BDD7-4A57-AAC9-88F94584ED79}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>No</t>
   </si>
@@ -106,13 +105,25 @@
   </si>
   <si>
     <t>Periode Semester</t>
+  </si>
+  <si>
+    <t>Alamat</t>
+  </si>
+  <si>
+    <t>Jl Srengseng Raya 88, Dki Jakarta</t>
+  </si>
+  <si>
+    <t>Jl Prof Dr Sudarto 126 A, Jawa Tengah</t>
+  </si>
+  <si>
+    <t>JL Pemuda No.1-G, Rawamangun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +156,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -199,6 +216,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,26 +534,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98D490D-845C-4710-A7F1-294360057CD8}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="28.88671875" customWidth="1"/>
-    <col min="7" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="9" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -552,19 +573,22 @@
         <v>22</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.6">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -583,20 +607,23 @@
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -615,20 +642,23 @@
       <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.6">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -647,27 +677,31 @@
       <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.6">
+    <row r="5" spans="1:11" ht="15.75">
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="15.6">
+    <row r="6" spans="1:11" ht="15.75">
       <c r="D6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>